<commit_message>
Báo cáo cuối kì lần 1
</commit_message>
<xml_diff>
--- a/Documents/TongHop/CK/01_Documents/DefinitionOfDone.xlsx
+++ b/Documents/TongHop/CK/01_Documents/DefinitionOfDone.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9192"/>
   </bookViews>
   <sheets>
-    <sheet name="Stories" sheetId="1" r:id="rId1"/>
+    <sheet name="Báo cáo" sheetId="2" r:id="rId1"/>
+    <sheet name="Stories" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="87">
   <si>
     <t>Là người dùng tôi muốn đăng ký tài khoản để bắt đầu theo dõi quá trình học</t>
   </si>
@@ -228,6 +229,63 @@
   </si>
   <si>
     <t>Sprint 13</t>
+  </si>
+  <si>
+    <t>Danh sách các báo cáo</t>
+  </si>
+  <si>
+    <t>Review</t>
+  </si>
+  <si>
+    <t>Project Vision</t>
+  </si>
+  <si>
+    <t>Project Charter</t>
+  </si>
+  <si>
+    <t>Executive Summary</t>
+  </si>
+  <si>
+    <t>Mockup</t>
+  </si>
+  <si>
+    <t>High level architect</t>
+  </si>
+  <si>
+    <t>Định nghĩa qui trình phần mềm</t>
+  </si>
+  <si>
+    <t>Product backlog</t>
+  </si>
+  <si>
+    <t>Bùi Đăng Khoa, Trần Hữu Nghĩa, Huỳnh Quang Minh</t>
+  </si>
+  <si>
+    <t>Danh sách rủi ro</t>
+  </si>
+  <si>
+    <t>Ước lượng thời gian, chi phí, công việc</t>
+  </si>
+  <si>
+    <t>Bùi Đăng Khoa, Trần Hữu Nghĩa</t>
+  </si>
+  <si>
+    <t>Báo cáo tình trạng</t>
+  </si>
+  <si>
+    <t>Release plan</t>
+  </si>
+  <si>
+    <t>Tài liệu hướng dẫn cài đặt, triền khai hệ thống</t>
+  </si>
+  <si>
+    <t>Tài liệu hướng dẫn sử dụng</t>
+  </si>
+  <si>
+    <t>Tài liệu hướng dẫn cài đặt môi trường, biên dịch mã nguồn</t>
+  </si>
+  <si>
+    <t>Các biên bản cuộc họp</t>
   </si>
 </sst>
 </file>
@@ -314,7 +372,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -365,12 +423,25 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.249977111117893"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -411,6 +482,10 @@
     <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Neutral" xfId="1" builtinId="28"/>
@@ -1752,10 +1827,469 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E38"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="68.5546875" customWidth="1"/>
+    <col min="2" max="2" width="48.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" customWidth="1"/>
+    <col min="4" max="4" width="16.109375" customWidth="1"/>
+    <col min="5" max="5" width="13" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="27" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>28</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>69</v>
+      </c>
+      <c r="D1" s="27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="27" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="16" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="16" t="s">
+        <v>71</v>
+      </c>
+      <c r="B3" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="16" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E8" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>77</v>
+      </c>
+      <c r="C9" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D9" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E10" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="24" t="s">
+        <v>79</v>
+      </c>
+      <c r="B11" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C11" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D11" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="24" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="24" t="s">
+        <v>82</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D13" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="24" t="s">
+        <v>83</v>
+      </c>
+      <c r="B14" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="B15" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C15" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A16" s="24" t="s">
+        <v>85</v>
+      </c>
+      <c r="B16" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="24" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="25">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D17" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="E17" s="17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="26"/>
+    </row>
+    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="26"/>
+    </row>
+    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="26"/>
+    </row>
+    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="1"/>
+      <c r="D21" s="1"/>
+      <c r="E21" s="26"/>
+    </row>
+    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="1"/>
+      <c r="D22" s="1"/>
+      <c r="E22" s="26"/>
+    </row>
+    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="26"/>
+    </row>
+    <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="26"/>
+    </row>
+    <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="26"/>
+    </row>
+    <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="26"/>
+    </row>
+    <row r="27" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M8" sqref="M8"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>